<commit_message>
Updated Stats - Wk 13
</commit_message>
<xml_diff>
--- a/FFStats.xlsx
+++ b/FFStats.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="62">
   <si>
     <t>Team</t>
   </si>
@@ -211,6 +211,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.000"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -253,8 +256,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -264,15 +269,17 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -605,9 +612,9 @@
   <dimension ref="A1:AO11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4740" topLeftCell="D1" activePane="topRight"/>
+      <pane xSplit="4740" topLeftCell="Z1" activePane="topRight"/>
       <selection activeCell="V2" sqref="V2"/>
-      <selection pane="topRight" activeCell="L16" sqref="L16"/>
+      <selection pane="topRight" activeCell="AN12" sqref="AN12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -764,14 +771,14 @@
       </c>
       <c r="H2">
         <f>SUM(N2:AA2)</f>
-        <v>1419.5</v>
+        <v>1585.5</v>
       </c>
       <c r="I2">
         <f>SUM(AB2:AP2)</f>
-        <v>1270</v>
+        <v>1357</v>
       </c>
       <c r="J2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K2">
         <v>6</v>
@@ -781,7 +788,7 @@
       </c>
       <c r="M2" s="1">
         <f>(J2+0.5*L2)/(J2+K2+L2)</f>
-        <v>0.5</v>
+        <v>0.53846153846153844</v>
       </c>
       <c r="N2">
         <v>141.5</v>
@@ -819,8 +826,8 @@
       <c r="Y2">
         <v>107</v>
       </c>
-      <c r="Z2" t="s">
-        <v>43</v>
+      <c r="Z2">
+        <v>166</v>
       </c>
       <c r="AA2" t="s">
         <v>43</v>
@@ -861,8 +868,8 @@
       <c r="AM2">
         <v>115.5</v>
       </c>
-      <c r="AN2" t="s">
-        <v>43</v>
+      <c r="AN2">
+        <v>87</v>
       </c>
       <c r="AO2" t="s">
         <v>43</v>
@@ -885,31 +892,31 @@
         <v>36</v>
       </c>
       <c r="F3">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G3">
         <v>7</v>
       </c>
       <c r="H3">
         <f t="shared" ref="H3:H11" si="0">SUM(N3:AA3)</f>
-        <v>1421.5</v>
+        <v>1508.5</v>
       </c>
       <c r="I3">
         <f t="shared" ref="I3:I11" si="1">SUM(AB3:AP3)</f>
-        <v>1480.5</v>
+        <v>1646.5</v>
       </c>
       <c r="J3">
         <v>5</v>
       </c>
       <c r="K3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="L3">
         <v>0</v>
       </c>
       <c r="M3" s="1">
         <f t="shared" ref="M3:M11" si="2">(J3+0.5*L3)/(J3+K3+L3)</f>
-        <v>0.41666666666666669</v>
+        <v>0.38461538461538464</v>
       </c>
       <c r="N3">
         <v>122.5</v>
@@ -947,8 +954,8 @@
       <c r="Y3">
         <v>119</v>
       </c>
-      <c r="Z3" t="s">
-        <v>43</v>
+      <c r="Z3">
+        <v>87</v>
       </c>
       <c r="AA3" t="s">
         <v>43</v>
@@ -989,8 +996,8 @@
       <c r="AM3">
         <v>129</v>
       </c>
-      <c r="AN3" t="s">
-        <v>43</v>
+      <c r="AN3">
+        <v>166</v>
       </c>
       <c r="AO3" t="s">
         <v>43</v>
@@ -1013,21 +1020,21 @@
         <v>25</v>
       </c>
       <c r="F4">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G4">
         <v>3</v>
       </c>
       <c r="H4">
         <f t="shared" si="0"/>
-        <v>1498</v>
+        <v>1680.5</v>
       </c>
       <c r="I4">
         <f t="shared" si="1"/>
-        <v>1387</v>
+        <v>1523</v>
       </c>
       <c r="J4">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="K4">
         <v>5</v>
@@ -1037,7 +1044,7 @@
       </c>
       <c r="M4" s="1">
         <f t="shared" si="2"/>
-        <v>0.58333333333333337</v>
+        <v>0.61538461538461542</v>
       </c>
       <c r="N4">
         <v>129.5</v>
@@ -1075,8 +1082,8 @@
       <c r="Y4">
         <v>127</v>
       </c>
-      <c r="Z4" t="s">
-        <v>43</v>
+      <c r="Z4">
+        <v>182.5</v>
       </c>
       <c r="AA4" t="s">
         <v>43</v>
@@ -1117,8 +1124,8 @@
       <c r="AM4">
         <v>125.5</v>
       </c>
-      <c r="AN4" t="s">
-        <v>43</v>
+      <c r="AN4">
+        <v>136</v>
       </c>
       <c r="AO4" t="s">
         <v>43</v>
@@ -1135,37 +1142,37 @@
         <v>3</v>
       </c>
       <c r="D5">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E5">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F5">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="G5">
         <v>4</v>
       </c>
       <c r="H5">
         <f t="shared" si="0"/>
-        <v>1369</v>
+        <v>1486.5</v>
       </c>
       <c r="I5">
         <f t="shared" si="1"/>
-        <v>1428.5</v>
+        <v>1565.5</v>
       </c>
       <c r="J5">
         <v>6</v>
       </c>
       <c r="K5">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L5">
         <v>0</v>
       </c>
       <c r="M5" s="1">
         <f t="shared" si="2"/>
-        <v>0.5</v>
+        <v>0.46153846153846156</v>
       </c>
       <c r="N5">
         <v>81.5</v>
@@ -1203,8 +1210,8 @@
       <c r="Y5">
         <v>129</v>
       </c>
-      <c r="Z5" t="s">
-        <v>43</v>
+      <c r="Z5">
+        <v>117.5</v>
       </c>
       <c r="AA5" t="s">
         <v>43</v>
@@ -1245,8 +1252,8 @@
       <c r="AM5">
         <v>119</v>
       </c>
-      <c r="AN5" t="s">
-        <v>43</v>
+      <c r="AN5">
+        <v>137</v>
       </c>
       <c r="AO5" t="s">
         <v>43</v>
@@ -1269,31 +1276,31 @@
         <v>28</v>
       </c>
       <c r="F6">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G6">
         <v>6</v>
       </c>
       <c r="H6">
         <f t="shared" si="0"/>
-        <v>1156.5</v>
+        <v>1218</v>
       </c>
       <c r="I6">
         <f t="shared" si="1"/>
-        <v>1340.5</v>
+        <v>1474.5</v>
       </c>
       <c r="J6">
         <v>5</v>
       </c>
       <c r="K6">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="L6">
         <v>0</v>
       </c>
       <c r="M6" s="1">
         <f t="shared" si="2"/>
-        <v>0.41666666666666669</v>
+        <v>0.38461538461538464</v>
       </c>
       <c r="N6">
         <v>103.5</v>
@@ -1331,8 +1338,8 @@
       <c r="Y6">
         <v>120</v>
       </c>
-      <c r="Z6" t="s">
-        <v>43</v>
+      <c r="Z6">
+        <v>61.5</v>
       </c>
       <c r="AA6" t="s">
         <v>43</v>
@@ -1373,8 +1380,8 @@
       <c r="AM6">
         <v>103</v>
       </c>
-      <c r="AN6" t="s">
-        <v>43</v>
+      <c r="AN6">
+        <v>134</v>
       </c>
       <c r="AO6" t="s">
         <v>43</v>
@@ -1397,21 +1404,21 @@
         <v>26</v>
       </c>
       <c r="F7">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G7">
         <v>1</v>
       </c>
       <c r="H7">
         <f t="shared" si="0"/>
-        <v>1350.5</v>
+        <v>1484.5</v>
       </c>
       <c r="I7">
         <f t="shared" si="1"/>
-        <v>1470.5</v>
+        <v>1532</v>
       </c>
       <c r="J7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K7">
         <v>7</v>
@@ -1421,7 +1428,7 @@
       </c>
       <c r="M7" s="1">
         <f t="shared" si="2"/>
-        <v>0.375</v>
+        <v>0.42307692307692307</v>
       </c>
       <c r="N7">
         <v>102.5</v>
@@ -1459,8 +1466,8 @@
       <c r="Y7">
         <v>115.5</v>
       </c>
-      <c r="Z7" t="s">
-        <v>43</v>
+      <c r="Z7">
+        <v>134</v>
       </c>
       <c r="AA7" t="s">
         <v>43</v>
@@ -1501,8 +1508,8 @@
       <c r="AM7">
         <v>107</v>
       </c>
-      <c r="AN7" t="s">
-        <v>43</v>
+      <c r="AN7">
+        <v>61.5</v>
       </c>
       <c r="AO7" t="s">
         <v>43</v>
@@ -1532,14 +1539,14 @@
       </c>
       <c r="H8">
         <f t="shared" si="0"/>
-        <v>1502.5</v>
+        <v>1644.5</v>
       </c>
       <c r="I8">
         <f t="shared" si="1"/>
-        <v>1385</v>
+        <v>1454.5</v>
       </c>
       <c r="J8">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="K8">
         <v>4</v>
@@ -1549,7 +1556,7 @@
       </c>
       <c r="M8" s="1">
         <f t="shared" si="2"/>
-        <v>0.625</v>
+        <v>0.65384615384615385</v>
       </c>
       <c r="N8">
         <v>155</v>
@@ -1587,8 +1594,8 @@
       <c r="Y8">
         <v>125.5</v>
       </c>
-      <c r="Z8" t="s">
-        <v>43</v>
+      <c r="Z8">
+        <v>142</v>
       </c>
       <c r="AA8" t="s">
         <v>43</v>
@@ -1629,8 +1636,8 @@
       <c r="AM8">
         <v>127</v>
       </c>
-      <c r="AN8" t="s">
-        <v>43</v>
+      <c r="AN8">
+        <v>69.5</v>
       </c>
       <c r="AO8" t="s">
         <v>43</v>
@@ -1660,24 +1667,24 @@
       </c>
       <c r="H9">
         <f t="shared" si="0"/>
-        <v>1358.5</v>
+        <v>1428</v>
       </c>
       <c r="I9">
         <f t="shared" si="1"/>
-        <v>1427.5</v>
+        <v>1569.5</v>
       </c>
       <c r="J9">
         <v>5</v>
       </c>
       <c r="K9">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="L9">
         <v>0</v>
       </c>
       <c r="M9" s="1">
         <f t="shared" si="2"/>
-        <v>0.41666666666666669</v>
+        <v>0.38461538461538464</v>
       </c>
       <c r="N9">
         <v>128.5</v>
@@ -1715,8 +1722,8 @@
       <c r="Y9">
         <v>103</v>
       </c>
-      <c r="Z9" t="s">
-        <v>43</v>
+      <c r="Z9">
+        <v>69.5</v>
       </c>
       <c r="AA9" t="s">
         <v>43</v>
@@ -1757,8 +1764,8 @@
       <c r="AM9">
         <v>120</v>
       </c>
-      <c r="AN9" t="s">
-        <v>43</v>
+      <c r="AN9">
+        <v>142</v>
       </c>
       <c r="AO9" t="s">
         <v>43</v>
@@ -1781,31 +1788,31 @@
         <v>14</v>
       </c>
       <c r="F10">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="G10">
         <v>0</v>
       </c>
       <c r="H10">
         <f t="shared" si="0"/>
-        <v>1437</v>
+        <v>1573</v>
       </c>
       <c r="I10">
         <f t="shared" si="1"/>
-        <v>1322</v>
+        <v>1504.5</v>
       </c>
       <c r="J10">
         <v>8</v>
       </c>
       <c r="K10">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L10">
         <v>0</v>
       </c>
       <c r="M10" s="1">
         <f t="shared" si="2"/>
-        <v>0.66666666666666663</v>
+        <v>0.61538461538461542</v>
       </c>
       <c r="N10">
         <v>109</v>
@@ -1843,8 +1850,8 @@
       <c r="Y10">
         <v>131.5</v>
       </c>
-      <c r="Z10" t="s">
-        <v>43</v>
+      <c r="Z10">
+        <v>136</v>
       </c>
       <c r="AA10" t="s">
         <v>43</v>
@@ -1885,8 +1892,8 @@
       <c r="AM10">
         <v>115.5</v>
       </c>
-      <c r="AN10" t="s">
-        <v>43</v>
+      <c r="AN10">
+        <v>182.5</v>
       </c>
       <c r="AO10" t="s">
         <v>43</v>
@@ -1903,27 +1910,27 @@
         <v>2</v>
       </c>
       <c r="D11">
+        <v>32</v>
+      </c>
+      <c r="E11">
         <v>31</v>
       </c>
-      <c r="E11">
-        <v>30</v>
-      </c>
       <c r="F11">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G11">
         <v>2</v>
       </c>
       <c r="H11">
         <f t="shared" si="0"/>
-        <v>1392.5</v>
+        <v>1529.5</v>
       </c>
       <c r="I11">
         <f t="shared" si="1"/>
-        <v>1388.5</v>
+        <v>1506</v>
       </c>
       <c r="J11">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K11">
         <v>6</v>
@@ -1933,7 +1940,7 @@
       </c>
       <c r="M11" s="1">
         <f t="shared" si="2"/>
-        <v>0.5</v>
+        <v>0.53846153846153844</v>
       </c>
       <c r="N11">
         <v>124.5</v>
@@ -1971,8 +1978,8 @@
       <c r="Y11">
         <v>115.5</v>
       </c>
-      <c r="Z11" t="s">
-        <v>43</v>
+      <c r="Z11">
+        <v>137</v>
       </c>
       <c r="AA11" t="s">
         <v>43</v>
@@ -2013,16 +2020,16 @@
       <c r="AM11">
         <v>131.5</v>
       </c>
-      <c r="AN11" t="s">
-        <v>43</v>
+      <c r="AN11">
+        <v>117.5</v>
       </c>
       <c r="AO11" t="s">
         <v>43</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="B24:G33">
-    <sortCondition ref="B23"/>
+  <sortState ref="B22:G31">
+    <sortCondition ref="B21"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Updated to include week 14 stats
</commit_message>
<xml_diff>
--- a/FFStats.xlsx
+++ b/FFStats.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
   <si>
     <t>Team</t>
   </si>
@@ -148,9 +148,6 @@
   </si>
   <si>
     <t>Emmett</t>
-  </si>
-  <si>
-    <t>NA</t>
   </si>
   <si>
     <t>A Nasty Moses</t>
@@ -212,7 +209,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -256,8 +253,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -269,17 +268,19 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -612,9 +613,9 @@
   <dimension ref="A1:AO11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4740" topLeftCell="Z1" activePane="topRight"/>
+      <pane xSplit="4740" activePane="topRight"/>
       <selection activeCell="V2" sqref="V2"/>
-      <selection pane="topRight" activeCell="AN12" sqref="AN12"/>
+      <selection pane="topRight" activeCell="AO11" sqref="AO11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -758,27 +759,27 @@
         <v>0</v>
       </c>
       <c r="D2">
+        <v>42</v>
+      </c>
+      <c r="E2">
         <v>40</v>
       </c>
-      <c r="E2">
-        <v>38</v>
-      </c>
       <c r="F2">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G2">
         <v>2</v>
       </c>
       <c r="H2">
         <f>SUM(N2:AA2)</f>
-        <v>1585.5</v>
+        <v>1707.5</v>
       </c>
       <c r="I2">
         <f>SUM(AB2:AP2)</f>
-        <v>1357</v>
+        <v>1469.5</v>
       </c>
       <c r="J2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="K2">
         <v>6</v>
@@ -788,7 +789,7 @@
       </c>
       <c r="M2" s="1">
         <f>(J2+0.5*L2)/(J2+K2+L2)</f>
-        <v>0.53846153846153844</v>
+        <v>0.5714285714285714</v>
       </c>
       <c r="N2">
         <v>141.5</v>
@@ -829,8 +830,8 @@
       <c r="Z2">
         <v>166</v>
       </c>
-      <c r="AA2" t="s">
-        <v>43</v>
+      <c r="AA2">
+        <v>122</v>
       </c>
       <c r="AB2">
         <v>155</v>
@@ -871,16 +872,16 @@
       <c r="AN2">
         <v>87</v>
       </c>
-      <c r="AO2" t="s">
-        <v>43</v>
+      <c r="AO2">
+        <v>112.5</v>
       </c>
     </row>
     <row r="3" spans="1:41">
       <c r="A3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" t="s">
         <v>44</v>
-      </c>
-      <c r="B3" t="s">
-        <v>45</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -892,31 +893,31 @@
         <v>36</v>
       </c>
       <c r="F3">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="G3">
         <v>7</v>
       </c>
       <c r="H3">
         <f t="shared" ref="H3:H11" si="0">SUM(N3:AA3)</f>
-        <v>1508.5</v>
+        <v>1578.5</v>
       </c>
       <c r="I3">
         <f t="shared" ref="I3:I11" si="1">SUM(AB3:AP3)</f>
-        <v>1646.5</v>
+        <v>1737</v>
       </c>
       <c r="J3">
         <v>5</v>
       </c>
       <c r="K3">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="L3">
         <v>0</v>
       </c>
       <c r="M3" s="1">
         <f t="shared" ref="M3:M11" si="2">(J3+0.5*L3)/(J3+K3+L3)</f>
-        <v>0.38461538461538464</v>
+        <v>0.35714285714285715</v>
       </c>
       <c r="N3">
         <v>122.5</v>
@@ -957,8 +958,8 @@
       <c r="Z3">
         <v>87</v>
       </c>
-      <c r="AA3" t="s">
-        <v>43</v>
+      <c r="AA3">
+        <v>70</v>
       </c>
       <c r="AB3">
         <v>124.5</v>
@@ -999,16 +1000,16 @@
       <c r="AN3">
         <v>166</v>
       </c>
-      <c r="AO3" t="s">
-        <v>43</v>
+      <c r="AO3">
+        <v>90.5</v>
       </c>
     </row>
     <row r="4" spans="1:41">
       <c r="A4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" t="s">
         <v>46</v>
-      </c>
-      <c r="B4" t="s">
-        <v>47</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -1027,14 +1028,14 @@
       </c>
       <c r="H4">
         <f t="shared" si="0"/>
-        <v>1680.5</v>
+        <v>1817.5</v>
       </c>
       <c r="I4">
         <f t="shared" si="1"/>
-        <v>1523</v>
+        <v>1615</v>
       </c>
       <c r="J4">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K4">
         <v>5</v>
@@ -1044,7 +1045,7 @@
       </c>
       <c r="M4" s="1">
         <f t="shared" si="2"/>
-        <v>0.61538461538461542</v>
+        <v>0.6428571428571429</v>
       </c>
       <c r="N4">
         <v>129.5</v>
@@ -1085,8 +1086,8 @@
       <c r="Z4">
         <v>182.5</v>
       </c>
-      <c r="AA4" t="s">
-        <v>43</v>
+      <c r="AA4">
+        <v>137</v>
       </c>
       <c r="AB4">
         <v>81.5</v>
@@ -1127,52 +1128,52 @@
       <c r="AN4">
         <v>136</v>
       </c>
-      <c r="AO4" t="s">
-        <v>43</v>
+      <c r="AO4">
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:41">
       <c r="A5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" t="s">
         <v>48</v>
-      </c>
-      <c r="B5" t="s">
-        <v>49</v>
       </c>
       <c r="C5">
         <v>3</v>
       </c>
       <c r="D5">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E5">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F5">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="G5">
         <v>4</v>
       </c>
       <c r="H5">
         <f t="shared" si="0"/>
-        <v>1486.5</v>
+        <v>1598.5</v>
       </c>
       <c r="I5">
         <f t="shared" si="1"/>
-        <v>1565.5</v>
+        <v>1687.5</v>
       </c>
       <c r="J5">
         <v>6</v>
       </c>
       <c r="K5">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="L5">
         <v>0</v>
       </c>
       <c r="M5" s="1">
         <f t="shared" si="2"/>
-        <v>0.46153846153846156</v>
+        <v>0.42857142857142855</v>
       </c>
       <c r="N5">
         <v>81.5</v>
@@ -1213,8 +1214,8 @@
       <c r="Z5">
         <v>117.5</v>
       </c>
-      <c r="AA5" t="s">
-        <v>43</v>
+      <c r="AA5">
+        <v>112</v>
       </c>
       <c r="AB5">
         <v>129.5</v>
@@ -1255,52 +1256,52 @@
       <c r="AN5">
         <v>137</v>
       </c>
-      <c r="AO5" t="s">
-        <v>43</v>
+      <c r="AO5">
+        <v>122</v>
       </c>
     </row>
     <row r="6" spans="1:41">
       <c r="A6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" t="s">
         <v>50</v>
-      </c>
-      <c r="B6" t="s">
-        <v>51</v>
       </c>
       <c r="C6">
         <v>2</v>
       </c>
       <c r="D6">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E6">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F6">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="G6">
         <v>6</v>
       </c>
       <c r="H6">
         <f t="shared" si="0"/>
-        <v>1218</v>
+        <v>1331.5</v>
       </c>
       <c r="I6">
         <f t="shared" si="1"/>
-        <v>1474.5</v>
+        <v>1617.5</v>
       </c>
       <c r="J6">
         <v>5</v>
       </c>
       <c r="K6">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="L6">
         <v>0</v>
       </c>
       <c r="M6" s="1">
         <f t="shared" si="2"/>
-        <v>0.38461538461538464</v>
+        <v>0.35714285714285715</v>
       </c>
       <c r="N6">
         <v>103.5</v>
@@ -1341,8 +1342,8 @@
       <c r="Z6">
         <v>61.5</v>
       </c>
-      <c r="AA6" t="s">
-        <v>43</v>
+      <c r="AA6">
+        <v>113.5</v>
       </c>
       <c r="AB6">
         <v>103.5</v>
@@ -1383,52 +1384,52 @@
       <c r="AN6">
         <v>134</v>
       </c>
-      <c r="AO6" t="s">
-        <v>43</v>
+      <c r="AO6">
+        <v>143</v>
       </c>
     </row>
     <row r="7" spans="1:41">
       <c r="A7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" t="s">
         <v>52</v>
-      </c>
-      <c r="B7" t="s">
-        <v>53</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E7">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F7">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="G7">
         <v>1</v>
       </c>
       <c r="H7">
         <f t="shared" si="0"/>
-        <v>1484.5</v>
+        <v>1562.5</v>
       </c>
       <c r="I7">
         <f t="shared" si="1"/>
-        <v>1532</v>
+        <v>1624.5</v>
       </c>
       <c r="J7">
         <v>5</v>
       </c>
       <c r="K7">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="L7">
         <v>1</v>
       </c>
       <c r="M7" s="1">
         <f t="shared" si="2"/>
-        <v>0.42307692307692307</v>
+        <v>0.39285714285714285</v>
       </c>
       <c r="N7">
         <v>102.5</v>
@@ -1469,8 +1470,8 @@
       <c r="Z7">
         <v>134</v>
       </c>
-      <c r="AA7" t="s">
-        <v>43</v>
+      <c r="AA7">
+        <v>78</v>
       </c>
       <c r="AB7">
         <v>128.5</v>
@@ -1511,42 +1512,42 @@
       <c r="AN7">
         <v>61.5</v>
       </c>
-      <c r="AO7" t="s">
-        <v>43</v>
+      <c r="AO7">
+        <v>92.5</v>
       </c>
     </row>
     <row r="8" spans="1:41">
       <c r="A8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" t="s">
         <v>54</v>
-      </c>
-      <c r="B8" t="s">
-        <v>55</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E8">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F8">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="G8">
         <v>6</v>
       </c>
       <c r="H8">
         <f t="shared" si="0"/>
-        <v>1644.5</v>
+        <v>1735</v>
       </c>
       <c r="I8">
         <f t="shared" si="1"/>
-        <v>1454.5</v>
+        <v>1524.5</v>
       </c>
       <c r="J8">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K8">
         <v>4</v>
@@ -1556,7 +1557,7 @@
       </c>
       <c r="M8" s="1">
         <f t="shared" si="2"/>
-        <v>0.65384615384615385</v>
+        <v>0.6785714285714286</v>
       </c>
       <c r="N8">
         <v>155</v>
@@ -1597,8 +1598,8 @@
       <c r="Z8">
         <v>142</v>
       </c>
-      <c r="AA8" t="s">
-        <v>43</v>
+      <c r="AA8">
+        <v>90.5</v>
       </c>
       <c r="AB8">
         <v>141.5</v>
@@ -1639,16 +1640,16 @@
       <c r="AN8">
         <v>69.5</v>
       </c>
-      <c r="AO8" t="s">
-        <v>43</v>
+      <c r="AO8">
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:41">
       <c r="A9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9" t="s">
         <v>56</v>
-      </c>
-      <c r="B9" t="s">
-        <v>57</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -1660,31 +1661,31 @@
         <v>21</v>
       </c>
       <c r="F9">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="G9">
         <v>3</v>
       </c>
       <c r="H9">
         <f t="shared" si="0"/>
-        <v>1428</v>
+        <v>1520</v>
       </c>
       <c r="I9">
         <f t="shared" si="1"/>
-        <v>1569.5</v>
+        <v>1706.5</v>
       </c>
       <c r="J9">
         <v>5</v>
       </c>
       <c r="K9">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="L9">
         <v>0</v>
       </c>
       <c r="M9" s="1">
         <f t="shared" si="2"/>
-        <v>0.38461538461538464</v>
+        <v>0.35714285714285715</v>
       </c>
       <c r="N9">
         <v>128.5</v>
@@ -1725,8 +1726,8 @@
       <c r="Z9">
         <v>69.5</v>
       </c>
-      <c r="AA9" t="s">
-        <v>43</v>
+      <c r="AA9">
+        <v>92</v>
       </c>
       <c r="AB9">
         <v>102.5</v>
@@ -1767,16 +1768,16 @@
       <c r="AN9">
         <v>142</v>
       </c>
-      <c r="AO9" t="s">
-        <v>43</v>
+      <c r="AO9">
+        <v>137</v>
       </c>
     </row>
     <row r="10" spans="1:41">
       <c r="A10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10" t="s">
         <v>58</v>
-      </c>
-      <c r="B10" t="s">
-        <v>59</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -1788,21 +1789,21 @@
         <v>14</v>
       </c>
       <c r="F10">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G10">
         <v>0</v>
       </c>
       <c r="H10">
         <f t="shared" si="0"/>
-        <v>1573</v>
+        <v>1665.5</v>
       </c>
       <c r="I10">
         <f t="shared" si="1"/>
-        <v>1504.5</v>
+        <v>1582.5</v>
       </c>
       <c r="J10">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K10">
         <v>5</v>
@@ -1812,7 +1813,7 @@
       </c>
       <c r="M10" s="1">
         <f t="shared" si="2"/>
-        <v>0.61538461538461542</v>
+        <v>0.6428571428571429</v>
       </c>
       <c r="N10">
         <v>109</v>
@@ -1853,8 +1854,8 @@
       <c r="Z10">
         <v>136</v>
       </c>
-      <c r="AA10" t="s">
-        <v>43</v>
+      <c r="AA10">
+        <v>92.5</v>
       </c>
       <c r="AB10">
         <v>103.5</v>
@@ -1895,42 +1896,42 @@
       <c r="AN10">
         <v>182.5</v>
       </c>
-      <c r="AO10" t="s">
-        <v>43</v>
+      <c r="AO10">
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:41">
       <c r="A11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11" t="s">
         <v>60</v>
-      </c>
-      <c r="B11" t="s">
-        <v>61</v>
       </c>
       <c r="C11">
         <v>2</v>
       </c>
       <c r="D11">
+        <v>33</v>
+      </c>
+      <c r="E11">
         <v>32</v>
       </c>
-      <c r="E11">
-        <v>31</v>
-      </c>
       <c r="F11">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="G11">
         <v>2</v>
       </c>
       <c r="H11">
         <f t="shared" si="0"/>
-        <v>1529.5</v>
+        <v>1672.5</v>
       </c>
       <c r="I11">
         <f t="shared" si="1"/>
-        <v>1506</v>
+        <v>1619.5</v>
       </c>
       <c r="J11">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="K11">
         <v>6</v>
@@ -1940,7 +1941,7 @@
       </c>
       <c r="M11" s="1">
         <f t="shared" si="2"/>
-        <v>0.53846153846153844</v>
+        <v>0.5714285714285714</v>
       </c>
       <c r="N11">
         <v>124.5</v>
@@ -1981,8 +1982,8 @@
       <c r="Z11">
         <v>137</v>
       </c>
-      <c r="AA11" t="s">
-        <v>43</v>
+      <c r="AA11">
+        <v>143</v>
       </c>
       <c r="AB11">
         <v>122.5</v>
@@ -2023,13 +2024,13 @@
       <c r="AN11">
         <v>117.5</v>
       </c>
-      <c r="AO11" t="s">
-        <v>43</v>
+      <c r="AO11">
+        <v>113.5</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="B22:G31">
-    <sortCondition ref="B21"/>
+  <sortState ref="C31:H40">
+    <sortCondition ref="C30"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>